<commit_message>
Korrekturen zur Übung vom 3.6.25
</commit_message>
<xml_diff>
--- a/Steuerlehre (B.A.) - Datenmanagement (dt)/uebungen/20250603_ETL_und_reporting_Excel/bank_transaktionen_q1_2024.xlsx
+++ b/Steuerlehre (B.A.) - Datenmanagement (dt)/uebungen/20250603_ETL_und_reporting_Excel/bank_transaktionen_q1_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/079e2bdfe6328f32/Dokumente/GitHub/DataManagement/Steuerlehre (B.A.) - Datenmanagement (dt)/uebungen/20250603_ETL_und_reporting_Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_9C281228E5D215E5E9ACF9D5CEFE60E15CE43F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F337EAE-2D50-4A1F-BD13-0F6A755B6ACC}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_9C281228E5D215E5E9ACF9D5CEFE60E15CE43F5B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{278F9343-A42F-437D-9E0C-7216603F8DB0}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4057" yWindow="4020" windowWidth="18225" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transaktionen" sheetId="1" r:id="rId1"/>
@@ -180,6 +180,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -383,9 +387,16 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.9296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">

</xml_diff>